<commit_message>
changed mpc direct aid arp
</commit_message>
<xml_diff>
--- a/results/01-2023/comparison-deflators-01-2023.xlsx
+++ b/results/01-2023/comparison-deflators-01-2023.xlsx
@@ -855,31 +855,31 @@
         <v>-0.0589</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0722</v>
+        <v>-0.0663</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0723</v>
+        <v>-0.0079</v>
       </c>
       <c r="L7" t="n">
-        <v>-0.0297</v>
+        <v>-0.0126</v>
       </c>
       <c r="M7" t="n">
-        <v>-0.0295</v>
+        <v>-0.0183</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.0517</v>
+        <v>-0.0516</v>
       </c>
       <c r="O7" t="n">
-        <v>-0.0741</v>
+        <v>0.0033</v>
       </c>
       <c r="P7" t="n">
-        <v>0.0335</v>
+        <v>0.0125</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.0321</v>
+        <v>0.012</v>
       </c>
       <c r="R7" t="n">
-        <v>0.0405</v>
+        <v>0.0213</v>
       </c>
     </row>
     <row r="8">
@@ -961,37 +961,37 @@
         <v>0.0342</v>
       </c>
       <c r="H9" t="n">
-        <v>-0.1402</v>
+        <v>-0.0637</v>
       </c>
       <c r="I9" t="n">
-        <v>-0.0911</v>
+        <v>-0.0648</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.0622</v>
+        <v>-0.0475</v>
       </c>
       <c r="K9" t="n">
-        <v>-0.0387</v>
+        <v>-0.1033</v>
       </c>
       <c r="L9" t="n">
-        <v>-0.0156</v>
+        <v>-0.0365</v>
       </c>
       <c r="M9" t="n">
-        <v>-0.0177</v>
+        <v>-0.0239</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.0394</v>
+        <v>-0.0264</v>
       </c>
       <c r="O9" t="n">
-        <v>-0.0343</v>
+        <v>-0.0206</v>
       </c>
       <c r="P9" t="n">
-        <v>-0.0284</v>
+        <v>-0.0218</v>
       </c>
       <c r="Q9" t="n">
-        <v>-0.0189</v>
+        <v>-0.0304</v>
       </c>
       <c r="R9" t="n">
-        <v>-0.0034</v>
+        <v>-0.0213</v>
       </c>
     </row>
     <row r="10">
@@ -1353,37 +1353,37 @@
         <v>-4.8306</v>
       </c>
       <c r="H16" t="n">
-        <v>-2.5625</v>
+        <v>-2.486</v>
       </c>
       <c r="I16" t="n">
-        <v>-1.0501</v>
+        <v>-1.0237</v>
       </c>
       <c r="J16" t="n">
-        <v>-1.4942</v>
+        <v>-1.4718</v>
       </c>
       <c r="K16" t="n">
-        <v>-2.3518</v>
+        <v>-1.7899</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.8729</v>
+        <v>-0.8836</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.6989</v>
+        <v>-0.7029</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.1566</v>
+        <v>-0.7425</v>
       </c>
       <c r="O16" t="n">
-        <v>-0.3425</v>
+        <v>-0.3441</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.313</v>
+        <v>-0.3357</v>
       </c>
       <c r="Q16" t="n">
-        <v>-0.048</v>
+        <v>-0.0937</v>
       </c>
       <c r="R16" t="n">
-        <v>0.0789</v>
+        <v>0.0342</v>
       </c>
     </row>
     <row r="17">
@@ -1586,25 +1586,25 @@
         <v>-0.0211</v>
       </c>
       <c r="K20" t="n">
-        <v>-1.0399</v>
+        <v>-0.4285</v>
       </c>
       <c r="L20" t="n">
-        <v>-0.0002</v>
+        <v>-0.0125</v>
       </c>
       <c r="M20" t="n">
-        <v>-0.0002</v>
+        <v>-0.0123</v>
       </c>
       <c r="N20" t="n">
-        <v>-0.0106</v>
+        <v>-0.6088</v>
       </c>
       <c r="O20" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P20" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="Q20" t="n">
-        <v>0</v>
+        <v>-0.0062</v>
       </c>
       <c r="R20" t="n">
         <v>0</v>
@@ -1807,31 +1807,31 @@
         <v>-0.0871</v>
       </c>
       <c r="J24" t="n">
-        <v>-0.0042</v>
+        <v>-0.0025</v>
       </c>
       <c r="K24" t="n">
-        <v>-0.0913</v>
+        <v>0.004</v>
       </c>
       <c r="L24" t="n">
-        <v>0.1147</v>
+        <v>0.12</v>
       </c>
       <c r="M24" t="n">
-        <v>0.1087</v>
+        <v>0.1118</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0955</v>
+        <v>0.0948</v>
       </c>
       <c r="O24" t="n">
-        <v>0.0826</v>
+        <v>-0.01</v>
       </c>
       <c r="P24" t="n">
-        <v>-0.059</v>
+        <v>-0.0672</v>
       </c>
       <c r="Q24" t="n">
-        <v>-0.0471</v>
+        <v>-0.055</v>
       </c>
       <c r="R24" t="n">
-        <v>-0.046</v>
+        <v>-0.0536</v>
       </c>
     </row>
     <row r="25">
@@ -2423,31 +2423,31 @@
         <v>0.0146</v>
       </c>
       <c r="J35" t="n">
-        <v>0.0117</v>
+        <v>0.0176</v>
       </c>
       <c r="K35" t="n">
-        <v>0.0087</v>
+        <v>-0.0715</v>
       </c>
       <c r="L35" t="n">
-        <v>0.0061</v>
+        <v>0.0232</v>
       </c>
       <c r="M35" t="n">
-        <v>-0.0082</v>
+        <v>0.003</v>
       </c>
       <c r="N35" t="n">
         <v>-0.0058</v>
       </c>
       <c r="O35" t="n">
-        <v>-0.0035</v>
+        <v>0.0739</v>
       </c>
       <c r="P35" t="n">
-        <v>-0.0014</v>
+        <v>-0.0224</v>
       </c>
       <c r="Q35" t="n">
-        <v>-0.0013</v>
+        <v>-0.0214</v>
       </c>
       <c r="R35" t="n">
-        <v>-0.0013</v>
+        <v>-0.0205</v>
       </c>
     </row>
     <row r="36">
@@ -2529,37 +2529,37 @@
         <v>0</v>
       </c>
       <c r="H37" t="n">
-        <v>0</v>
+        <v>0.0765</v>
       </c>
       <c r="I37" t="n">
-        <v>-0.0004</v>
+        <v>0.0259</v>
       </c>
       <c r="J37" t="n">
-        <v>0.0002</v>
+        <v>0.0149</v>
       </c>
       <c r="K37" t="n">
-        <v>0</v>
+        <v>-0.0646</v>
       </c>
       <c r="L37" t="n">
-        <v>0.0002</v>
+        <v>-0.0207</v>
       </c>
       <c r="M37" t="n">
-        <v>0</v>
+        <v>-0.0061</v>
       </c>
       <c r="N37" t="n">
-        <v>0</v>
+        <v>0.013</v>
       </c>
       <c r="O37" t="n">
-        <v>0</v>
+        <v>0.0137</v>
       </c>
       <c r="P37" t="n">
-        <v>0</v>
+        <v>0.0066</v>
       </c>
       <c r="Q37" t="n">
-        <v>0</v>
+        <v>-0.0115</v>
       </c>
       <c r="R37" t="n">
-        <v>0.0001</v>
+        <v>-0.0178</v>
       </c>
     </row>
     <row r="38">
@@ -2921,37 +2921,37 @@
         <v>0</v>
       </c>
       <c r="H44" t="n">
-        <v>0.0005</v>
+        <v>0.0769</v>
       </c>
       <c r="I44" t="n">
-        <v>1.0517</v>
+        <v>1.078</v>
       </c>
       <c r="J44" t="n">
-        <v>0.3384</v>
+        <v>0.3607</v>
       </c>
       <c r="K44" t="n">
-        <v>0.2001</v>
+        <v>0.7619</v>
       </c>
       <c r="L44" t="n">
-        <v>0.1913</v>
+        <v>0.1807</v>
       </c>
       <c r="M44" t="n">
-        <v>-0.2288</v>
+        <v>-0.2328</v>
       </c>
       <c r="N44" t="n">
-        <v>0.0116</v>
+        <v>-0.5743</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0256</v>
+        <v>0.024</v>
       </c>
       <c r="P44" t="n">
-        <v>0.0254</v>
+        <v>0.0026</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.0407</v>
+        <v>-0.0864</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.0364</v>
+        <v>-0.0811</v>
       </c>
     </row>
     <row r="45">
@@ -3154,25 +3154,25 @@
         <v>0</v>
       </c>
       <c r="K48" t="n">
-        <v>0.0007</v>
+        <v>0.6121</v>
       </c>
       <c r="L48" t="n">
-        <v>0</v>
+        <v>-0.0122</v>
       </c>
       <c r="M48" t="n">
-        <v>0</v>
+        <v>-0.0121</v>
       </c>
       <c r="N48" t="n">
-        <v>0</v>
+        <v>-0.5982</v>
       </c>
       <c r="O48" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="P48" t="n">
-        <v>0</v>
+        <v>-0.0001</v>
       </c>
       <c r="Q48" t="n">
-        <v>0</v>
+        <v>-0.0062</v>
       </c>
       <c r="R48" t="n">
         <v>0</v>
@@ -3375,31 +3375,31 @@
         <v>-0.0085</v>
       </c>
       <c r="J52" t="n">
-        <v>-0.0091</v>
+        <v>-0.0074</v>
       </c>
       <c r="K52" t="n">
-        <v>-0.0097</v>
+        <v>0.0856</v>
       </c>
       <c r="L52" t="n">
-        <v>-0.0106</v>
+        <v>-0.0053</v>
       </c>
       <c r="M52" t="n">
-        <v>-0.0022</v>
+        <v>0.0009</v>
       </c>
       <c r="N52" t="n">
-        <v>-0.0013</v>
+        <v>-0.002</v>
       </c>
       <c r="O52" t="n">
-        <v>-0.0004</v>
+        <v>-0.0929</v>
       </c>
       <c r="P52" t="n">
-        <v>0.0007</v>
+        <v>-0.0074</v>
       </c>
       <c r="Q52" t="n">
-        <v>0.0007</v>
+        <v>-0.0072</v>
       </c>
       <c r="R52" t="n">
-        <v>0.0007</v>
+        <v>-0.0069</v>
       </c>
     </row>
     <row r="53">

</xml_diff>